<commit_message>
Python fully automatic USB
.
</commit_message>
<xml_diff>
--- a/lookup_dataset.xlsx
+++ b/lookup_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\ardynamic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336D296D-0C20-4D90-BC31-CE780CAAD0C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8B1991-9085-4535-A93E-87D9A36C0DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3F4DC67-60B5-4F48-8657-29C3A7D1DDB2}"/>
   </bookViews>
@@ -227,12 +227,6 @@
     <t>x={0,1,2,….}, note: 0 and 1 is reserved for halt, others are reserved for which test to perform</t>
   </si>
   <si>
-    <t>Arduino only reads serial if it is halted, various test functions may exist</t>
-  </si>
-  <si>
-    <t>#000:002:XX$</t>
-  </si>
-  <si>
     <t>#002:003:XXX$</t>
   </si>
   <si>
@@ -959,6 +953,12 @@
   </si>
   <si>
     <t>T={0,1,2}, 0:reset both; 1:reset read; 2reset variable</t>
+  </si>
+  <si>
+    <t>#000:003:000$</t>
+  </si>
+  <si>
+    <t>Arduino prints ("#HELLO,ITS ME$")</t>
   </si>
 </sst>
 </file>
@@ -1581,8 +1581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02DAD5F2-9586-408C-B968-AE93F04DF7BB}">
   <dimension ref="B1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,18 +1599,18 @@
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -1638,19 +1638,19 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
@@ -1689,7 +1689,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>24</v>
@@ -1727,13 +1727,13 @@
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -1748,7 +1748,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>26</v>
@@ -1769,13 +1769,13 @@
         <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -1790,16 +1790,16 @@
         <v>6</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -1813,7 +1813,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>20</v>
@@ -1822,12 +1822,12 @@
         <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1">
         <v>9</v>
@@ -1836,7 +1836,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>17</v>
@@ -1845,12 +1845,12 @@
         <v>18</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1">
         <v>10</v>
@@ -1859,40 +1859,40 @@
         <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2">
         <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1">
         <v>12</v>
@@ -1901,19 +1901,19 @@
         <v>4</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1">
         <v>13</v>
@@ -1922,19 +1922,19 @@
         <v>4</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C19" s="23">
         <v>14</v>
@@ -1943,19 +1943,19 @@
         <v>2</v>
       </c>
       <c r="E19" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="G19" s="23" t="s">
         <v>124</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>126</v>
       </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C20" s="35">
         <v>15</v>
@@ -1964,17 +1964,17 @@
         <v>1</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G20" s="37"/>
       <c r="H20" s="22"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="36" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C21" s="35">
         <v>16</v>
@@ -1983,10 +1983,10 @@
         <v>1</v>
       </c>
       <c r="E21" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="F21" s="35" t="s">
         <v>132</v>
-      </c>
-      <c r="F21" s="35" t="s">
-        <v>134</v>
       </c>
       <c r="G21" s="37"/>
       <c r="H21" s="22"/>
@@ -1994,20 +1994,20 @@
     <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="5" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C5" s="23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="6" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C6" s="23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="8" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D8" s="24">
         <v>0</v>
@@ -2220,7 +2220,7 @@
     </row>
     <row r="9" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="1"/>
@@ -2317,7 +2317,7 @@
     <row r="16" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D17" s="24">
         <v>0</v>
@@ -2472,7 +2472,7 @@
     </row>
     <row r="18" spans="3:53" x14ac:dyDescent="0.25">
       <c r="C18" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>9</v>
@@ -2537,22 +2537,22 @@
     </row>
     <row r="19" spans="3:53" x14ac:dyDescent="0.25">
       <c r="C19" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2602,22 +2602,22 @@
     </row>
     <row r="20" spans="3:53" x14ac:dyDescent="0.25">
       <c r="C20" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2667,22 +2667,22 @@
     </row>
     <row r="21" spans="3:53" x14ac:dyDescent="0.25">
       <c r="C21" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2732,22 +2732,22 @@
     </row>
     <row r="22" spans="3:53" x14ac:dyDescent="0.25">
       <c r="C22" s="28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2797,7 +2797,7 @@
     </row>
     <row r="23" spans="3:53" x14ac:dyDescent="0.25">
       <c r="C23" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D23" s="24">
         <v>0</v>
@@ -2809,10 +2809,10 @@
         <v>2</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -2862,22 +2862,22 @@
     </row>
     <row r="24" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D24" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="G24" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2928,7 +2928,7 @@
     <row r="27" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D28" s="24">
         <v>0</v>
@@ -3083,25 +3083,25 @@
     </row>
     <row r="29" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D29" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -3151,7 +3151,7 @@
     <row r="32" spans="3:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D33" s="24">
         <v>0</v>
@@ -3306,22 +3306,22 @@
     </row>
     <row r="34" spans="2:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D34" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="G34" s="31" t="s">
         <v>107</v>
-      </c>
-      <c r="F34" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="G34" s="31" t="s">
-        <v>109</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -3372,7 +3372,7 @@
     </row>
     <row r="35" spans="2:53" x14ac:dyDescent="0.25">
       <c r="C35" s="28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D35" s="24"/>
       <c r="E35" s="1"/>
@@ -3427,7 +3427,7 @@
     </row>
     <row r="36" spans="2:53" x14ac:dyDescent="0.25">
       <c r="C36" s="28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="1"/>
@@ -3482,7 +3482,7 @@
     </row>
     <row r="37" spans="2:53" x14ac:dyDescent="0.25">
       <c r="C37" s="28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="1"/>
@@ -3537,7 +3537,7 @@
     </row>
     <row r="38" spans="2:53" x14ac:dyDescent="0.25">
       <c r="C38" s="28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D38" s="24"/>
       <c r="E38" s="1"/>
@@ -3592,7 +3592,7 @@
     </row>
     <row r="39" spans="2:53" x14ac:dyDescent="0.25">
       <c r="C39" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D39" s="24"/>
       <c r="E39" s="1"/>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="40" spans="2:53" x14ac:dyDescent="0.25">
       <c r="C40" s="28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D40" s="24"/>
       <c r="E40" s="1"/>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="41" spans="2:53" x14ac:dyDescent="0.25">
       <c r="C41" s="28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D41" s="24"/>
       <c r="E41" s="1"/>
@@ -3757,7 +3757,7 @@
     </row>
     <row r="42" spans="2:53" x14ac:dyDescent="0.25">
       <c r="C42" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D42" s="24"/>
       <c r="E42" s="1"/>
@@ -3812,7 +3812,7 @@
     </row>
     <row r="43" spans="2:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D43" s="24"/>
       <c r="E43" s="1"/>
@@ -3868,7 +3868,7 @@
     <row r="45" spans="2:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="2:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D46" s="24">
         <v>0</v>
@@ -3903,7 +3903,7 @@
     </row>
     <row r="47" spans="2:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D47" s="24">
         <v>4</v>
@@ -3939,7 +3939,7 @@
     <row r="48" spans="2:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D49" s="24">
         <v>0</v>
@@ -4095,7 +4095,7 @@
     </row>
     <row r="50" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C50" s="33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="1"/>
@@ -4150,7 +4150,7 @@
     </row>
     <row r="51" spans="3:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D51" s="24"/>
       <c r="E51" s="1"/>

</xml_diff>